<commit_message>
Atualização de metricas e sensores
</commit_message>
<xml_diff>
--- a/Pi/Documentação/METRICAS DOS SENSORES.xlsx
+++ b/Pi/Documentação/METRICAS DOS SENSORES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4924f6f5e1aaa61e/Área de Trabalho/Facul BandTec/Clones Git/Grupo-11--Microalgas/Pi/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\reposity-Gabriel\Grupo-11--Microalgas\Pi\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D6D5A74C-FB91-4E85-9C1C-C673D4AD7934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8AC5B158-47E2-4C2B-AF8A-A1F2D1F76124}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285F9F12-1351-467D-A1DE-8D704C47114D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{189BC5A4-360A-4B39-9270-63572D4582FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{189BC5A4-360A-4B39-9270-63572D4582FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>MIN</t>
   </si>
@@ -62,17 +62,17 @@
     <t>IDEAL</t>
   </si>
   <si>
-    <t>GRAFICO</t>
+    <t>METRICAS E ESTASTISTICAS</t>
   </si>
   <si>
-    <t>METRICAS E ESTASTISTICAS</t>
+    <t>GRÁFICO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +80,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,24 +113,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4B4B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -130,11 +171,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -145,24 +249,64 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF4B4B"/>
+      <color rgb="FFFF2929"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1151,7 +1295,7 @@
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>33336</xdr:rowOff>
@@ -1479,109 +1623,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87609DA-9815-47B4-AC57-059C61B7A2EB}">
-  <dimension ref="B2:K24"/>
+  <dimension ref="B2:T24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="5" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>0.25</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="8">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="8">
+        <v>30</v>
+      </c>
+      <c r="K5" s="15">
         <v>0.75</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="2">
         <v>21</v>
       </c>
-      <c r="E6" s="3">
-        <v>20</v>
+      <c r="E6" s="17">
+        <v>15</v>
       </c>
       <c r="F6" s="6">
         <f>_xlfn.QUARTILE.EXC(C5:C24,1)</f>
         <v>21.5</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="9"/>
+      <c r="H6" s="3">
         <f>AVERAGE(C5:C24)</f>
         <v>24.85</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="3">
         <f>MEDIAN(C5:C24)</f>
         <v>25.5</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="9"/>
+      <c r="K6" s="14">
         <f>_xlfn.QUARTILE.EXC(C5:C24,3)</f>
         <v>27.75</v>
       </c>
-      <c r="J6" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -1589,24 +1742,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2">
         <v>26</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>5</v>
       </c>
@@ -1614,7 +1769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -1622,15 +1777,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -1638,7 +1794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>9</v>
       </c>
@@ -1646,7 +1802,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>10</v>
       </c>
@@ -1654,7 +1810,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>11</v>
       </c>
@@ -1662,7 +1818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>12</v>
       </c>
@@ -1735,11 +1891,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E8:K8"/>
+  <mergeCells count="5">
+    <mergeCell ref="E8:M8"/>
     <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>